<commit_message>
update schematic: add io expander with peripherals, update power circuitry- change some components. update project plan. update footprints
</commit_message>
<xml_diff>
--- a/hardware/ESP32 Pin Allocation.xlsx
+++ b/hardware/ESP32 Pin Allocation.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD06F1CF-53F6-4E90-BBB6-2288D968ABFA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFED3C11-4A24-4DA7-A204-3879F7955F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32 GPIO" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -378,7 +377,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="145">
   <si>
     <t>Wroom32</t>
   </si>
@@ -810,6 +809,9 @@
   </si>
   <si>
     <t>OLED SDA</t>
+  </si>
+  <si>
+    <t>OLED addr = 0x3C</t>
   </si>
 </sst>
 </file>
@@ -1256,8 +1258,8 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2844,7 +2846,9 @@
         <v>143</v>
       </c>
       <c r="N35" s="12"/>
-      <c r="P35" s="11"/>
+      <c r="P35" s="11" t="s">
+        <v>144</v>
+      </c>
       <c r="Q35" s="21"/>
       <c r="R35" s="11"/>
       <c r="S35" s="3"/>

</xml_diff>

<commit_message>
update footprints for 24way connector, 3D models. add new connector to connect the two PCB's
</commit_message>
<xml_diff>
--- a/hardware/ESP32 Pin Allocation.xlsx
+++ b/hardware/ESP32 Pin Allocation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhan.charler\Documents\Projects\hardware\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFED3C11-4A24-4DA7-A204-3879F7955F4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A8474F-70D5-47DC-926F-CFD1C111F5A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32 GPIO" sheetId="1" r:id="rId1"/>
@@ -377,7 +377,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="146">
   <si>
     <t>Wroom32</t>
   </si>
@@ -813,12 +813,15 @@
   <si>
     <t>OLED addr = 0x3C</t>
   </si>
+  <si>
+    <t>IO expander address [7:0] = 0 1 0 0 A2 A1 A0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -849,12 +852,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="-webkit-standard"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF1155CC"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -978,7 +975,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1022,19 +1019,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1259,7 +1255,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1325,7 +1321,7 @@
       <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="Q1" s="27" t="s">
         <v>111</v>
       </c>
       <c r="R1" s="3"/>
@@ -1510,7 +1506,7 @@
       <c r="L5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="29" t="s">
         <v>139</v>
       </c>
       <c r="N5" s="12"/>
@@ -1566,7 +1562,7 @@
       </c>
       <c r="N6" s="12"/>
       <c r="P6" s="11"/>
-      <c r="Q6" s="27"/>
+      <c r="Q6" s="26"/>
       <c r="R6" s="3"/>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
@@ -1614,10 +1610,10 @@
         <v>120</v>
       </c>
       <c r="N7" s="12"/>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="Q7" s="27" t="s">
+      <c r="Q7" s="26" t="s">
         <v>142</v>
       </c>
       <c r="R7" s="3"/>
@@ -1952,7 +1948,7 @@
       </c>
       <c r="N15" s="12"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="27" t="s">
+      <c r="Q15" s="26" t="s">
         <v>110</v>
       </c>
       <c r="R15" s="3"/>
@@ -2003,7 +1999,7 @@
       <c r="P16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q16" s="27" t="s">
+      <c r="Q16" s="26" t="s">
         <v>110</v>
       </c>
       <c r="R16" s="3"/>
@@ -2100,7 +2096,7 @@
         <v>125</v>
       </c>
       <c r="N18" s="12"/>
-      <c r="P18" s="28" t="s">
+      <c r="P18" s="27" t="s">
         <v>107</v>
       </c>
       <c r="R18" s="3"/>
@@ -2146,7 +2142,7 @@
         <v>126</v>
       </c>
       <c r="N19" s="12"/>
-      <c r="P19" s="28" t="s">
+      <c r="P19" s="27" t="s">
         <v>107</v>
       </c>
       <c r="Q19" s="3"/>
@@ -2209,7 +2205,7 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" ht="14.4" customHeight="1">
+    <row r="21" spans="1:30" ht="22.2" customHeight="1">
       <c r="A21" s="4">
         <v>31</v>
       </c>
@@ -2842,14 +2838,16 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="31" t="s">
+      <c r="M35" s="30" t="s">
         <v>143</v>
       </c>
       <c r="N35" s="12"/>
       <c r="P35" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="Q35" s="21"/>
+      <c r="Q35" t="s">
+        <v>145</v>
+      </c>
       <c r="R35" s="11"/>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
@@ -3023,7 +3021,7 @@
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="N39" s="12"/>
-      <c r="P39" s="22" t="s">
+      <c r="P39" s="21" t="s">
         <v>83</v>
       </c>
       <c r="Q39" s="11"/>
@@ -3063,7 +3061,7 @@
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="N40" s="12"/>
-      <c r="P40" s="22" t="s">
+      <c r="P40" s="21" t="s">
         <v>83</v>
       </c>
       <c r="Q40" s="11"/>
@@ -3163,17 +3161,17 @@
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="N43" s="29" t="s">
+      <c r="N43" s="28" t="s">
         <v>109</v>
       </c>
       <c r="P43" s="3"/>
@@ -3259,7 +3257,7 @@
     </row>
     <row r="46" spans="1:30" ht="13.2">
       <c r="A46" s="3"/>
-      <c r="B46" s="25"/>
+      <c r="B46" s="24"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -3289,7 +3287,7 @@
       <c r="AD46" s="3"/>
     </row>
     <row r="47" spans="1:30" ht="13.2">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="26" t="s">
         <v>106</v>
       </c>
       <c r="B47" s="9"/>

</xml_diff>